<commit_message>
Subset Analysis written and completed
</commit_message>
<xml_diff>
--- a/Assignment2CombinedResults.xlsx
+++ b/Assignment2CombinedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaleb\Documents\GitHub\ECE614Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE7D21A8-62B2-4285-A9E6-BD4C5626122D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B0ACA3-F774-482A-B111-3B800D3594E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="540" windowWidth="25590" windowHeight="16740" activeTab="2" xr2:uid="{0C750C2F-5C0E-432E-8ABE-5463668D346D}"/>
+    <workbookView xWindow="150" yWindow="195" windowWidth="13530" windowHeight="18285" activeTab="2" xr2:uid="{0C750C2F-5C0E-432E-8ABE-5463668D346D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 &amp; 2" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
   <dimension ref="A1:E602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10810,8 +10810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27195E5-F9F2-4B17-8404-B90328E09D0B}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13223,8 +13223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE370D3-6420-4750-8737-028301178E3A}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>